<commit_message>
Added new data (post-publication)
</commit_message>
<xml_diff>
--- a/HF_means_sd.xlsx
+++ b/HF_means_sd.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="50">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -124,6 +124,9 @@
     <t xml:space="preserve">Wifi</t>
   </si>
   <si>
+    <t xml:space="preserve">Bumblebee</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mason bee</t>
   </si>
   <si>
@@ -140,9 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">Wasp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taye2017</t>
   </si>
   <si>
     <t xml:space="preserve">Stever2006</t>
@@ -170,12 +170,6 @@
   </si>
   <si>
     <t xml:space="preserve">Treder2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cappucci2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drosophila</t>
   </si>
 </sst>
 </file>
@@ -258,7 +252,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,10 +270,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -406,12 +396,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M181"/>
+  <dimension ref="A1:M178"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A101" activeCellId="0" sqref="A101"/>
+      <selection pane="bottomLeft" activeCell="A178" activeCellId="0" sqref="178:178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2914,7 +2904,7 @@
         <v>34</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="E66" s="3" t="n">
         <f aca="false">2*30*24</f>
@@ -2922,26 +2912,27 @@
       </c>
       <c r="F66" s="4" t="n">
         <f aca="false">(I66/J66)-1</f>
-        <v>0.483050847457627</v>
+        <v>-0.0307167235494882</v>
       </c>
       <c r="G66" s="1" t="n">
-        <v>431</v>
+        <v>4</v>
       </c>
       <c r="H66" s="1" t="n">
-        <v>426</v>
-      </c>
-      <c r="I66" s="1" t="n">
-        <v>17.5</v>
+        <v>4</v>
+      </c>
+      <c r="I66" s="3" t="n">
+        <v>56.8</v>
       </c>
       <c r="J66" s="1" t="n">
-        <v>11.8</v>
-      </c>
-      <c r="K66" s="1" t="n">
-        <v>8.55</v>
+        <v>58.6</v>
+      </c>
+      <c r="K66" s="3" t="n">
+        <v>44.5</v>
       </c>
       <c r="L66" s="1" t="n">
-        <v>3.66</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="M66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
@@ -2951,10 +2942,10 @@
         <v>33</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>0.87</v>
+        <v>2.13</v>
       </c>
       <c r="E67" s="3" t="n">
         <f aca="false">2*30*24</f>
@@ -2962,22 +2953,22 @@
       </c>
       <c r="F67" s="4" t="n">
         <f aca="false">(I67/J67)-1</f>
-        <v>0.338983050847458</v>
+        <v>0.483050847457627</v>
       </c>
       <c r="G67" s="1" t="n">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="H67" s="1" t="n">
         <v>426</v>
       </c>
-      <c r="I67" s="3" t="n">
-        <v>15.8</v>
+      <c r="I67" s="1" t="n">
+        <v>17.5</v>
       </c>
       <c r="J67" s="1" t="n">
         <v>11.8</v>
       </c>
       <c r="K67" s="1" t="n">
-        <v>3.08</v>
+        <v>8.55</v>
       </c>
       <c r="L67" s="1" t="n">
         <v>3.66</v>
@@ -2991,10 +2982,10 @@
         <v>33</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>0.55</v>
+        <v>0.87</v>
       </c>
       <c r="E68" s="3" t="n">
         <f aca="false">2*30*24</f>
@@ -3002,22 +2993,22 @@
       </c>
       <c r="F68" s="4" t="n">
         <f aca="false">(I68/J68)-1</f>
-        <v>0.0847457627118644</v>
+        <v>0.338983050847458</v>
       </c>
       <c r="G68" s="1" t="n">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="H68" s="1" t="n">
         <v>426</v>
       </c>
       <c r="I68" s="3" t="n">
-        <v>12.8</v>
+        <v>15.8</v>
       </c>
       <c r="J68" s="1" t="n">
         <v>11.8</v>
       </c>
       <c r="K68" s="1" t="n">
-        <v>4.62</v>
+        <v>3.08</v>
       </c>
       <c r="L68" s="1" t="n">
         <v>3.66</v>
@@ -3028,39 +3019,39 @@
         <v>32</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>0.857</v>
-      </c>
-      <c r="E69" s="1" t="n">
-        <f aca="false">120*24</f>
-        <v>2880</v>
+        <v>0.55</v>
+      </c>
+      <c r="E69" s="3" t="n">
+        <f aca="false">2*30*24</f>
+        <v>1440</v>
       </c>
       <c r="F69" s="4" t="n">
         <f aca="false">(I69/J69)-1</f>
-        <v>1.84779050736498</v>
+        <v>0.0847457627118644</v>
       </c>
       <c r="G69" s="1" t="n">
-        <v>152</v>
+        <v>433</v>
       </c>
       <c r="H69" s="1" t="n">
-        <v>594</v>
-      </c>
-      <c r="I69" s="1" t="n">
-        <v>17.4</v>
+        <v>426</v>
+      </c>
+      <c r="I69" s="3" t="n">
+        <v>12.8</v>
       </c>
       <c r="J69" s="1" t="n">
-        <v>6.11</v>
+        <v>11.8</v>
       </c>
       <c r="K69" s="1" t="n">
-        <v>8.03</v>
+        <v>4.62</v>
       </c>
       <c r="L69" s="1" t="n">
-        <v>11.7</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3071,10 +3062,10 @@
         <v>30</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>0.562</v>
+        <v>0.857</v>
       </c>
       <c r="E70" s="1" t="n">
         <f aca="false">120*24</f>
@@ -3082,22 +3073,22 @@
       </c>
       <c r="F70" s="4" t="n">
         <f aca="false">(I70/J70)-1</f>
-        <v>0.543371522094926</v>
+        <v>1.84779050736498</v>
       </c>
       <c r="G70" s="1" t="n">
-        <v>447</v>
+        <v>152</v>
       </c>
       <c r="H70" s="1" t="n">
         <v>594</v>
       </c>
-      <c r="I70" s="3" t="n">
-        <v>9.43</v>
+      <c r="I70" s="1" t="n">
+        <v>17.4</v>
       </c>
       <c r="J70" s="1" t="n">
         <v>6.11</v>
       </c>
       <c r="K70" s="1" t="n">
-        <v>13.6</v>
+        <v>8.03</v>
       </c>
       <c r="L70" s="1" t="n">
         <v>11.7</v>
@@ -3111,10 +3102,10 @@
         <v>30</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>0.391</v>
+        <v>0.562</v>
       </c>
       <c r="E71" s="1" t="n">
         <f aca="false">120*24</f>
@@ -3122,69 +3113,70 @@
       </c>
       <c r="F71" s="4" t="n">
         <f aca="false">(I71/J71)-1</f>
-        <v>0.176759410801964</v>
+        <v>0.543371522094926</v>
       </c>
       <c r="G71" s="1" t="n">
-        <v>649</v>
+        <v>447</v>
       </c>
       <c r="H71" s="1" t="n">
         <v>594</v>
       </c>
       <c r="I71" s="3" t="n">
-        <v>7.19</v>
+        <v>9.43</v>
       </c>
       <c r="J71" s="1" t="n">
         <v>6.11</v>
       </c>
       <c r="K71" s="1" t="n">
-        <v>8.92</v>
+        <v>13.6</v>
       </c>
       <c r="L71" s="1" t="n">
         <v>11.7</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D72" s="2" t="n">
-        <v>4.21</v>
+      <c r="D72" s="1" t="n">
+        <v>0.391</v>
       </c>
       <c r="E72" s="1" t="n">
-        <v>8</v>
+        <f aca="false">120*24</f>
+        <v>2880</v>
       </c>
       <c r="F72" s="4" t="n">
         <f aca="false">(I72/J72)-1</f>
-        <v>0.25</v>
+        <v>0.176759410801964</v>
       </c>
       <c r="G72" s="1" t="n">
-        <v>228</v>
+        <v>649</v>
       </c>
       <c r="H72" s="1" t="n">
-        <v>158</v>
+        <v>594</v>
       </c>
       <c r="I72" s="3" t="n">
-        <v>15</v>
+        <v>7.19</v>
       </c>
       <c r="J72" s="1" t="n">
-        <v>12</v>
+        <v>6.11</v>
       </c>
       <c r="K72" s="1" t="n">
-        <v>5</v>
+        <v>8.92</v>
       </c>
       <c r="L72" s="1" t="n">
-        <v>5</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>23</v>
@@ -3200,30 +3192,30 @@
       </c>
       <c r="F73" s="4" t="n">
         <f aca="false">(I73/J73)-1</f>
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G73" s="1" t="n">
-        <v>345</v>
+        <v>228</v>
       </c>
       <c r="H73" s="1" t="n">
-        <v>266</v>
-      </c>
-      <c r="I73" s="1" t="n">
-        <v>4</v>
+        <v>158</v>
+      </c>
+      <c r="I73" s="3" t="n">
+        <v>15</v>
       </c>
       <c r="J73" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K73" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L73" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>23</v>
@@ -3239,30 +3231,30 @@
       </c>
       <c r="F74" s="4" t="n">
         <f aca="false">(I74/J74)-1</f>
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="G74" s="1" t="n">
-        <v>176</v>
+        <v>345</v>
       </c>
       <c r="H74" s="1" t="n">
-        <v>125</v>
+        <v>266</v>
       </c>
       <c r="I74" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J74" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K74" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J74" s="1" t="n">
+      <c r="L74" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="K74" s="1" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="L74" s="1" t="n">
-        <v>3.5</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>23</v>
@@ -3278,30 +3270,30 @@
       </c>
       <c r="F75" s="4" t="n">
         <f aca="false">(I75/J75)-1</f>
+        <v>-0.25</v>
+      </c>
+      <c r="G75" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="H75" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="I75" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G75" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="H75" s="1" t="n">
-        <v>193</v>
-      </c>
-      <c r="I75" s="1" t="n">
-        <v>20</v>
-      </c>
       <c r="J75" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K75" s="1" t="n">
-        <v>6</v>
+        <v>2.5</v>
       </c>
       <c r="L75" s="1" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>23</v>
@@ -3313,11 +3305,11 @@
         <v>4.21</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F76" s="4" t="n">
         <f aca="false">(I76/J76)-1</f>
-        <v>0.357142857142857</v>
+        <v>3</v>
       </c>
       <c r="G76" s="1" t="n">
         <v>200</v>
@@ -3326,76 +3318,76 @@
         <v>193</v>
       </c>
       <c r="I76" s="1" t="n">
-        <v>9.5</v>
+        <v>20</v>
       </c>
       <c r="J76" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K76" s="1" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="L76" s="1" t="n">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D77" s="1" t="n">
-        <v>1.27913</v>
+        <v>31</v>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>4.21</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="F77" s="4" t="n">
         <f aca="false">(I77/J77)-1</f>
-        <v>0.0400916380297822</v>
+        <v>0.357142857142857</v>
       </c>
       <c r="G77" s="1" t="n">
-        <v>5</v>
+        <v>200</v>
       </c>
       <c r="H77" s="1" t="n">
-        <v>5</v>
+        <v>193</v>
       </c>
       <c r="I77" s="1" t="n">
-        <v>9.08</v>
+        <v>9.5</v>
       </c>
       <c r="J77" s="1" t="n">
-        <v>8.73</v>
+        <v>7</v>
       </c>
       <c r="K77" s="1" t="n">
-        <v>2.63</v>
+        <v>3.5</v>
       </c>
       <c r="L77" s="1" t="n">
-        <v>2.39</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>0.33349</v>
+        <v>1.27913</v>
       </c>
       <c r="E78" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F78" s="4" t="n">
         <f aca="false">(I78/J78)-1</f>
-        <v>0.130570758405004</v>
+        <v>0.0400916380297822</v>
       </c>
       <c r="G78" s="1" t="n">
         <v>5</v>
@@ -3404,37 +3396,37 @@
         <v>5</v>
       </c>
       <c r="I78" s="1" t="n">
-        <v>14.46</v>
+        <v>9.08</v>
       </c>
       <c r="J78" s="1" t="n">
-        <v>12.79</v>
+        <v>8.73</v>
       </c>
       <c r="K78" s="1" t="n">
-        <v>4.42</v>
+        <v>2.63</v>
       </c>
       <c r="L78" s="1" t="n">
-        <v>4.9</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>0.38978</v>
+        <v>0.33349</v>
       </c>
       <c r="E79" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F79" s="4" t="n">
         <f aca="false">(I79/J79)-1</f>
-        <v>1.13428120063191</v>
+        <v>0.130570758405004</v>
       </c>
       <c r="G79" s="1" t="n">
         <v>5</v>
@@ -3443,37 +3435,37 @@
         <v>5</v>
       </c>
       <c r="I79" s="1" t="n">
-        <v>13.51</v>
+        <v>14.46</v>
       </c>
       <c r="J79" s="1" t="n">
-        <v>6.33</v>
+        <v>12.79</v>
       </c>
       <c r="K79" s="1" t="n">
-        <v>2.15</v>
+        <v>4.42</v>
       </c>
       <c r="L79" s="1" t="n">
-        <v>2.28</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>0.31667</v>
+        <v>0.38978</v>
       </c>
       <c r="E80" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F80" s="4" t="n">
         <f aca="false">(I80/J80)-1</f>
-        <v>-0.396635679504205</v>
+        <v>1.13428120063191</v>
       </c>
       <c r="G80" s="1" t="n">
         <v>5</v>
@@ -3482,37 +3474,37 @@
         <v>5</v>
       </c>
       <c r="I80" s="1" t="n">
-        <v>13.63</v>
+        <v>13.51</v>
       </c>
       <c r="J80" s="1" t="n">
-        <v>22.59</v>
+        <v>6.33</v>
       </c>
       <c r="K80" s="1" t="n">
-        <v>3.94</v>
+        <v>2.15</v>
       </c>
       <c r="L80" s="1" t="n">
-        <v>4.3</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>0.43199</v>
+        <v>0.31667</v>
       </c>
       <c r="E81" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F81" s="4" t="n">
         <f aca="false">(I81/J81)-1</f>
-        <v>-0.169240669240669</v>
+        <v>-0.396635679504205</v>
       </c>
       <c r="G81" s="1" t="n">
         <v>5</v>
@@ -3521,37 +3513,37 @@
         <v>5</v>
       </c>
       <c r="I81" s="1" t="n">
-        <v>12.91</v>
+        <v>13.63</v>
       </c>
       <c r="J81" s="1" t="n">
-        <v>15.54</v>
+        <v>22.59</v>
       </c>
       <c r="K81" s="1" t="n">
-        <v>6.45</v>
+        <v>3.94</v>
       </c>
       <c r="L81" s="1" t="n">
-        <v>7.41</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>0.22138</v>
+        <v>0.43199</v>
       </c>
       <c r="E82" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F82" s="4" t="n">
         <f aca="false">(I82/J82)-1</f>
-        <v>-0.144089732528041</v>
+        <v>-0.169240669240669</v>
       </c>
       <c r="G82" s="1" t="n">
         <v>5</v>
@@ -3560,21 +3552,21 @@
         <v>5</v>
       </c>
       <c r="I82" s="1" t="n">
-        <v>9.92</v>
+        <v>12.91</v>
       </c>
       <c r="J82" s="1" t="n">
-        <v>11.59</v>
+        <v>15.54</v>
       </c>
       <c r="K82" s="1" t="n">
-        <v>2.87</v>
+        <v>6.45</v>
       </c>
       <c r="L82" s="1" t="n">
-        <v>3.47</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>30</v>
@@ -3583,54 +3575,53 @@
         <v>38</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>1.27913</v>
+        <v>0.22138</v>
       </c>
       <c r="E83" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F83" s="4" t="n">
         <f aca="false">(I83/J83)-1</f>
-        <v>-0.713238024507984</v>
+        <v>-0.144089732528041</v>
       </c>
       <c r="G83" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H83" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I83" s="1" t="n">
-        <v>3.089</v>
+        <v>9.92</v>
       </c>
       <c r="J83" s="1" t="n">
-        <v>10.772</v>
+        <v>11.59</v>
       </c>
       <c r="K83" s="1" t="n">
-        <v>0.951</v>
+        <v>2.87</v>
       </c>
       <c r="L83" s="1" t="n">
-        <v>5.703</v>
-      </c>
-      <c r="M83" s="4"/>
+        <v>3.47</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>0.33349</v>
+        <v>1.27913</v>
       </c>
       <c r="E84" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F84" s="4" t="n">
         <f aca="false">(I84/J84)-1</f>
-        <v>0.28062015503876</v>
+        <v>-0.713238024507984</v>
       </c>
       <c r="G84" s="1" t="n">
         <v>6</v>
@@ -3639,37 +3630,38 @@
         <v>6</v>
       </c>
       <c r="I84" s="1" t="n">
-        <v>5.782</v>
+        <v>3.089</v>
       </c>
       <c r="J84" s="1" t="n">
-        <v>4.515</v>
+        <v>10.772</v>
       </c>
       <c r="K84" s="1" t="n">
-        <v>4.04</v>
+        <v>0.951</v>
       </c>
       <c r="L84" s="1" t="n">
-        <v>2.693</v>
-      </c>
+        <v>5.703</v>
+      </c>
+      <c r="M84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>0.38978</v>
+        <v>0.33349</v>
       </c>
       <c r="E85" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F85" s="4" t="n">
         <f aca="false">(I85/J85)-1</f>
-        <v>0.250060694343287</v>
+        <v>0.28062015503876</v>
       </c>
       <c r="G85" s="1" t="n">
         <v>6</v>
@@ -3678,37 +3670,37 @@
         <v>6</v>
       </c>
       <c r="I85" s="1" t="n">
-        <v>5.149</v>
+        <v>5.782</v>
       </c>
       <c r="J85" s="1" t="n">
-        <v>4.119</v>
+        <v>4.515</v>
       </c>
       <c r="K85" s="1" t="n">
-        <v>2.376</v>
+        <v>4.04</v>
       </c>
       <c r="L85" s="1" t="n">
-        <v>0.871</v>
+        <v>2.693</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>0.31667</v>
+        <v>0.38978</v>
       </c>
       <c r="E86" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F86" s="4" t="n">
         <f aca="false">(I86/J86)-1</f>
-        <v>-0.565672022443254</v>
+        <v>0.250060694343287</v>
       </c>
       <c r="G86" s="1" t="n">
         <v>6</v>
@@ -3717,37 +3709,37 @@
         <v>6</v>
       </c>
       <c r="I86" s="1" t="n">
-        <v>3.406</v>
+        <v>5.149</v>
       </c>
       <c r="J86" s="1" t="n">
-        <v>7.842</v>
+        <v>4.119</v>
       </c>
       <c r="K86" s="1" t="n">
-        <v>1.346</v>
+        <v>2.376</v>
       </c>
       <c r="L86" s="1" t="n">
-        <v>1.742</v>
+        <v>0.871</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>0.43199</v>
+        <v>0.31667</v>
       </c>
       <c r="E87" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F87" s="4" t="n">
         <f aca="false">(I87/J87)-1</f>
-        <v>-0.535617673579802</v>
+        <v>-0.565672022443254</v>
       </c>
       <c r="G87" s="1" t="n">
         <v>6</v>
@@ -3756,37 +3748,37 @@
         <v>6</v>
       </c>
       <c r="I87" s="1" t="n">
-        <v>1.03</v>
+        <v>3.406</v>
       </c>
       <c r="J87" s="1" t="n">
-        <v>2.218</v>
+        <v>7.842</v>
       </c>
       <c r="K87" s="1" t="n">
-        <v>0.713</v>
+        <v>1.346</v>
       </c>
       <c r="L87" s="1" t="n">
-        <v>1.03</v>
+        <v>1.742</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>0.22138</v>
+        <v>0.43199</v>
       </c>
       <c r="E88" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F88" s="4" t="n">
         <f aca="false">(I88/J88)-1</f>
-        <v>-0.166705634790741</v>
+        <v>-0.535617673579802</v>
       </c>
       <c r="G88" s="1" t="n">
         <v>6</v>
@@ -3795,21 +3787,21 @@
         <v>6</v>
       </c>
       <c r="I88" s="1" t="n">
-        <v>3.564</v>
+        <v>1.03</v>
       </c>
       <c r="J88" s="1" t="n">
-        <v>4.277</v>
+        <v>2.218</v>
       </c>
       <c r="K88" s="1" t="n">
-        <v>1.426</v>
+        <v>0.713</v>
       </c>
       <c r="L88" s="1" t="n">
-        <v>2.218</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>30</v>
@@ -3818,53 +3810,53 @@
         <v>39</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>1.27913</v>
+        <v>0.22138</v>
       </c>
       <c r="E89" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F89" s="4" t="n">
         <f aca="false">(I89/J89)-1</f>
-        <v>-0.27608863694924</v>
+        <v>-0.166705634790741</v>
       </c>
       <c r="G89" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H89" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I89" s="1" t="n">
-        <v>56.19</v>
+        <v>3.564</v>
       </c>
       <c r="J89" s="1" t="n">
-        <v>77.62</v>
+        <v>4.277</v>
       </c>
       <c r="K89" s="1" t="n">
-        <v>29.52</v>
+        <v>1.426</v>
       </c>
       <c r="L89" s="1" t="n">
-        <v>20.48</v>
+        <v>2.218</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>0.33349</v>
+        <v>1.27913</v>
       </c>
       <c r="E90" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F90" s="4" t="n">
         <f aca="false">(I90/J90)-1</f>
-        <v>-0.0595000000000001</v>
+        <v>-0.27608863694924</v>
       </c>
       <c r="G90" s="1" t="n">
         <v>5</v>
@@ -3873,37 +3865,37 @@
         <v>5</v>
       </c>
       <c r="I90" s="1" t="n">
-        <v>75.24</v>
+        <v>56.19</v>
       </c>
       <c r="J90" s="1" t="n">
-        <v>80</v>
+        <v>77.62</v>
       </c>
       <c r="K90" s="1" t="n">
-        <v>20.47</v>
+        <v>29.52</v>
       </c>
       <c r="L90" s="1" t="n">
-        <v>16.67</v>
+        <v>20.48</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>0.38978</v>
+        <v>0.33349</v>
       </c>
       <c r="E91" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F91" s="4" t="n">
         <f aca="false">(I91/J91)-1</f>
-        <v>0.136875</v>
+        <v>-0.0595000000000001</v>
       </c>
       <c r="G91" s="1" t="n">
         <v>5</v>
@@ -3912,37 +3904,37 @@
         <v>5</v>
       </c>
       <c r="I91" s="1" t="n">
-        <v>90.95</v>
+        <v>75.24</v>
       </c>
       <c r="J91" s="1" t="n">
         <v>80</v>
       </c>
       <c r="K91" s="1" t="n">
-        <v>9.53</v>
+        <v>20.47</v>
       </c>
       <c r="L91" s="1" t="n">
-        <v>11.43</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D92" s="1" t="n">
-        <v>0.31667</v>
+        <v>0.38978</v>
       </c>
       <c r="E92" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F92" s="4" t="n">
         <f aca="false">(I92/J92)-1</f>
-        <v>0.181881291218327</v>
+        <v>0.136875</v>
       </c>
       <c r="G92" s="1" t="n">
         <v>5</v>
@@ -3951,37 +3943,37 @@
         <v>5</v>
       </c>
       <c r="I92" s="1" t="n">
-        <v>68.1</v>
+        <v>90.95</v>
       </c>
       <c r="J92" s="1" t="n">
-        <v>57.62</v>
+        <v>80</v>
       </c>
       <c r="K92" s="1" t="n">
-        <v>16.19</v>
+        <v>9.53</v>
       </c>
       <c r="L92" s="1" t="n">
-        <v>19.05</v>
+        <v>11.43</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D93" s="1" t="n">
-        <v>0.43199</v>
+        <v>0.31667</v>
       </c>
       <c r="E93" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F93" s="4" t="n">
         <f aca="false">(I93/J93)-1</f>
-        <v>-0.101926163723917</v>
+        <v>0.181881291218327</v>
       </c>
       <c r="G93" s="1" t="n">
         <v>5</v>
@@ -3990,37 +3982,37 @@
         <v>5</v>
       </c>
       <c r="I93" s="1" t="n">
-        <v>67.14</v>
+        <v>68.1</v>
       </c>
       <c r="J93" s="1" t="n">
-        <v>74.76</v>
+        <v>57.62</v>
       </c>
       <c r="K93" s="1" t="n">
-        <v>13.34</v>
+        <v>16.19</v>
       </c>
       <c r="L93" s="1" t="n">
-        <v>16.19</v>
+        <v>19.05</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D94" s="1" t="n">
-        <v>0.22138</v>
+        <v>0.43199</v>
       </c>
       <c r="E94" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F94" s="4" t="n">
         <f aca="false">(I94/J94)-1</f>
-        <v>-0.0190058479532163</v>
+        <v>-0.101926163723917</v>
       </c>
       <c r="G94" s="1" t="n">
         <v>5</v>
@@ -4029,60 +4021,60 @@
         <v>5</v>
       </c>
       <c r="I94" s="1" t="n">
-        <v>73.81</v>
+        <v>67.14</v>
       </c>
       <c r="J94" s="1" t="n">
-        <v>75.24</v>
+        <v>74.76</v>
       </c>
       <c r="K94" s="1" t="n">
-        <v>12.86</v>
+        <v>13.34</v>
       </c>
       <c r="L94" s="1" t="n">
-        <v>7.62</v>
+        <v>16.19</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D95" s="1" t="n">
-        <v>1.27913</v>
+        <v>0.22138</v>
       </c>
       <c r="E95" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F95" s="4" t="n">
         <f aca="false">(I95/J95)-1</f>
-        <v>0.138528138528139</v>
+        <v>-0.0190058479532163</v>
       </c>
       <c r="G95" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H95" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I95" s="1" t="n">
-        <v>131.5</v>
+        <v>73.81</v>
       </c>
       <c r="J95" s="1" t="n">
-        <v>115.5</v>
+        <v>75.24</v>
       </c>
       <c r="K95" s="1" t="n">
-        <v>150.6</v>
+        <v>12.86</v>
       </c>
       <c r="L95" s="1" t="n">
-        <v>133.9</v>
+        <v>7.62</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>30</v>
@@ -4091,14 +4083,14 @@
         <v>14</v>
       </c>
       <c r="D96" s="1" t="n">
-        <v>0.33349</v>
+        <v>1.27913</v>
       </c>
       <c r="E96" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F96" s="4" t="n">
         <f aca="false">(I96/J96)-1</f>
-        <v>0.0721903199343723</v>
+        <v>0.138528138528139</v>
       </c>
       <c r="G96" s="1" t="n">
         <v>9</v>
@@ -4107,21 +4099,21 @@
         <v>9</v>
       </c>
       <c r="I96" s="1" t="n">
-        <v>130.7</v>
+        <v>131.5</v>
       </c>
       <c r="J96" s="1" t="n">
-        <v>121.9</v>
+        <v>115.5</v>
       </c>
       <c r="K96" s="1" t="n">
         <v>150.6</v>
       </c>
       <c r="L96" s="1" t="n">
-        <v>139.4</v>
+        <v>133.9</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>30</v>
@@ -4130,14 +4122,14 @@
         <v>14</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>0.38978</v>
+        <v>0.33349</v>
       </c>
       <c r="E97" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F97" s="4" t="n">
         <f aca="false">(I97/J97)-1</f>
-        <v>0.3301775147929</v>
+        <v>0.0721903199343723</v>
       </c>
       <c r="G97" s="1" t="n">
         <v>9</v>
@@ -4146,21 +4138,21 @@
         <v>9</v>
       </c>
       <c r="I97" s="1" t="n">
-        <v>112.4</v>
+        <v>130.7</v>
       </c>
       <c r="J97" s="1" t="n">
-        <v>84.5</v>
+        <v>121.9</v>
       </c>
       <c r="K97" s="1" t="n">
-        <v>137.8</v>
+        <v>150.6</v>
       </c>
       <c r="L97" s="1" t="n">
-        <v>115.5</v>
+        <v>139.4</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>30</v>
@@ -4169,14 +4161,14 @@
         <v>14</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>0.31667</v>
+        <v>0.38978</v>
       </c>
       <c r="E98" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F98" s="4" t="n">
         <f aca="false">(I98/J98)-1</f>
-        <v>-0.371149511645379</v>
+        <v>0.3301775147929</v>
       </c>
       <c r="G98" s="1" t="n">
         <v>9</v>
@@ -4185,21 +4177,21 @@
         <v>9</v>
       </c>
       <c r="I98" s="1" t="n">
-        <v>83.7</v>
+        <v>112.4</v>
       </c>
       <c r="J98" s="1" t="n">
-        <v>133.1</v>
+        <v>84.5</v>
       </c>
       <c r="K98" s="1" t="n">
-        <v>130.7</v>
+        <v>137.8</v>
       </c>
       <c r="L98" s="1" t="n">
-        <v>151.4</v>
+        <v>115.5</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>30</v>
@@ -4208,14 +4200,14 @@
         <v>14</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>0.43199</v>
+        <v>0.31667</v>
       </c>
       <c r="E99" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F99" s="4" t="n">
         <f aca="false">(I99/J99)-1</f>
-        <v>-0.0331034482758622</v>
+        <v>-0.371149511645379</v>
       </c>
       <c r="G99" s="1" t="n">
         <v>9</v>
@@ -4224,21 +4216,21 @@
         <v>9</v>
       </c>
       <c r="I99" s="1" t="n">
-        <v>140.2</v>
+        <v>83.7</v>
       </c>
       <c r="J99" s="1" t="n">
-        <v>145</v>
+        <v>133.1</v>
       </c>
       <c r="K99" s="1" t="n">
-        <v>148.2</v>
+        <v>130.7</v>
       </c>
       <c r="L99" s="1" t="n">
-        <v>154.6</v>
+        <v>151.4</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>30</v>
@@ -4247,14 +4239,14 @@
         <v>14</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>0.22138</v>
+        <v>0.43199</v>
       </c>
       <c r="E100" s="1" t="n">
         <v>48</v>
       </c>
       <c r="F100" s="4" t="n">
         <f aca="false">(I100/J100)-1</f>
-        <v>-0.236842105263158</v>
+        <v>-0.0331034482758622</v>
       </c>
       <c r="G100" s="1" t="n">
         <v>9</v>
@@ -4263,244 +4255,236 @@
         <v>9</v>
       </c>
       <c r="I100" s="1" t="n">
+        <v>140.2</v>
+      </c>
+      <c r="J100" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="K100" s="1" t="n">
+        <v>148.2</v>
+      </c>
+      <c r="L100" s="1" t="n">
+        <v>154.6</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" s="1" t="n">
+        <v>0.22138</v>
+      </c>
+      <c r="E101" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="F101" s="4" t="n">
+        <f aca="false">(I101/J101)-1</f>
+        <v>-0.236842105263158</v>
+      </c>
+      <c r="G101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="I101" s="1" t="n">
         <v>113.1</v>
       </c>
-      <c r="J100" s="1" t="n">
+      <c r="J101" s="1" t="n">
         <v>148.2</v>
       </c>
-      <c r="K100" s="1" t="n">
+      <c r="K101" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="L100" s="1" t="n">
+      <c r="L101" s="1" t="n">
         <v>157</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D101" s="1" t="n">
-        <v>0.174</v>
-      </c>
-      <c r="E101" s="1" t="n">
-        <v>4320</v>
-      </c>
-      <c r="F101" s="5" t="n">
-        <v>-0.096</v>
-      </c>
-      <c r="G101" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H101" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="I101" s="1" t="n">
-        <v>28.5828</v>
-      </c>
-      <c r="J101" s="1" t="n">
-        <v>32.4171</v>
-      </c>
-      <c r="K101" s="1" t="n">
-        <v>0.4714</v>
-      </c>
-      <c r="L101" s="1" t="n">
-        <v>1.0671</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D102" s="1" t="n">
-        <v>0.101</v>
+        <v>1.82143</v>
       </c>
       <c r="E102" s="1" t="n">
-        <v>4320</v>
+        <v>262</v>
       </c>
       <c r="F102" s="4" t="n">
-        <v>-0.082</v>
+        <v>-0.81</v>
       </c>
       <c r="G102" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H102" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I102" s="1" t="n">
-        <v>30.9585</v>
+        <v>3.37</v>
       </c>
       <c r="J102" s="1" t="n">
-        <v>32.4171</v>
+        <v>27.17</v>
       </c>
       <c r="K102" s="1" t="n">
-        <v>1.2367</v>
+        <v>15.63</v>
       </c>
       <c r="L102" s="1" t="n">
-        <v>1.0671</v>
+        <v>4.86</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D103" s="1" t="n">
-        <v>0.093</v>
+        <v>1.82143</v>
       </c>
       <c r="E103" s="1" t="n">
-        <v>4320</v>
+        <v>262</v>
       </c>
       <c r="F103" s="4" t="n">
-        <v>-0.015</v>
+        <v>-0.22</v>
       </c>
       <c r="G103" s="1" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="H103" s="1" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="I103" s="1" t="n">
-        <v>31.7085</v>
+        <v>38.48</v>
       </c>
       <c r="J103" s="1" t="n">
-        <v>32.4171</v>
+        <v>48.97</v>
       </c>
       <c r="K103" s="1" t="n">
-        <v>0.7694</v>
+        <v>16.41</v>
       </c>
       <c r="L103" s="1" t="n">
-        <v>1.0671</v>
+        <v>20.74</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D104" s="1" t="n">
-        <v>0.082</v>
+        <v>0.07</v>
       </c>
       <c r="E104" s="1" t="n">
-        <v>4320</v>
-      </c>
-      <c r="F104" s="4" t="n">
-        <v>0.033</v>
+        <v>336</v>
       </c>
       <c r="G104" s="1" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H104" s="1" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="I104" s="1" t="n">
-        <v>33.2914</v>
+        <v>0.16</v>
       </c>
       <c r="J104" s="1" t="n">
-        <v>32.4171</v>
+        <v>0.18</v>
       </c>
       <c r="K104" s="1" t="n">
-        <v>1.2781</v>
+        <v>0.02</v>
       </c>
       <c r="L104" s="1" t="n">
-        <v>1.0671</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D105" s="1" t="n">
-        <v>1.82143</v>
+        <v>0.07</v>
       </c>
       <c r="E105" s="1" t="n">
-        <v>262</v>
-      </c>
-      <c r="F105" s="4" t="n">
-        <v>-0.81</v>
+        <v>336</v>
       </c>
       <c r="G105" s="1" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H105" s="1" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="I105" s="1" t="n">
-        <v>3.37</v>
+        <v>0.18</v>
       </c>
       <c r="J105" s="1" t="n">
-        <v>27.17</v>
+        <v>0.26</v>
       </c>
       <c r="K105" s="1" t="n">
-        <v>15.63</v>
+        <v>0.004</v>
       </c>
       <c r="L105" s="1" t="n">
-        <v>4.86</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D106" s="1" t="n">
-        <v>1.82143</v>
+        <v>0.07</v>
       </c>
       <c r="E106" s="1" t="n">
-        <v>262</v>
-      </c>
-      <c r="F106" s="4" t="n">
-        <v>-0.22</v>
+        <v>336</v>
       </c>
       <c r="G106" s="1" t="n">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="H106" s="1" t="n">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="I106" s="1" t="n">
-        <v>38.48</v>
+        <v>0.04</v>
       </c>
       <c r="J106" s="1" t="n">
-        <v>48.97</v>
+        <v>0.04</v>
       </c>
       <c r="K106" s="1" t="n">
-        <v>16.41</v>
+        <v>0.003</v>
       </c>
       <c r="L106" s="1" t="n">
-        <v>20.74</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4514,7 +4498,7 @@
         <v>46</v>
       </c>
       <c r="D107" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E107" s="1" t="n">
         <v>336</v>
@@ -4526,7 +4510,7 @@
         <v>30</v>
       </c>
       <c r="I107" s="1" t="n">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="J107" s="1" t="n">
         <v>0.18</v>
@@ -4549,7 +4533,7 @@
         <v>47</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E108" s="1" t="n">
         <v>336</v>
@@ -4561,13 +4545,13 @@
         <v>20</v>
       </c>
       <c r="I108" s="1" t="n">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="J108" s="1" t="n">
         <v>0.26</v>
       </c>
       <c r="K108" s="1" t="n">
-        <v>0.004</v>
+        <v>0.01</v>
       </c>
       <c r="L108" s="1" t="n">
         <v>0.03</v>
@@ -4584,7 +4568,7 @@
         <v>48</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E109" s="1" t="n">
         <v>336</v>
@@ -4596,13 +4580,13 @@
         <v>50</v>
       </c>
       <c r="I109" s="1" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="J109" s="1" t="n">
         <v>0.04</v>
       </c>
       <c r="K109" s="1" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="L109" s="1" t="n">
         <v>0.01</v>
@@ -4619,10 +4603,10 @@
         <v>46</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E110" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G110" s="1" t="n">
         <v>30</v>
@@ -4631,16 +4615,16 @@
         <v>30</v>
       </c>
       <c r="I110" s="1" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="J110" s="1" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="K110" s="1" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="L110" s="1" t="n">
-        <v>0.004</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4654,10 +4638,10 @@
         <v>47</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E111" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G111" s="1" t="n">
         <v>20</v>
@@ -4666,16 +4650,16 @@
         <v>20</v>
       </c>
       <c r="I111" s="1" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="J111" s="1" t="n">
-        <v>0.26</v>
+        <v>0.29</v>
       </c>
       <c r="K111" s="1" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L111" s="1" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4689,10 +4673,10 @@
         <v>48</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E112" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G112" s="1" t="n">
         <v>50</v>
@@ -4701,16 +4685,16 @@
         <v>50</v>
       </c>
       <c r="I112" s="1" t="n">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="J112" s="1" t="n">
         <v>0.04</v>
       </c>
       <c r="K112" s="1" t="n">
-        <v>0.004</v>
+        <v>0.03</v>
       </c>
       <c r="L112" s="1" t="n">
-        <v>0.01</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4724,7 +4708,7 @@
         <v>46</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E113" s="1" t="n">
         <v>3360</v>
@@ -4736,7 +4720,7 @@
         <v>30</v>
       </c>
       <c r="I113" s="1" t="n">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="J113" s="1" t="n">
         <v>0.16</v>
@@ -4759,7 +4743,7 @@
         <v>47</v>
       </c>
       <c r="D114" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E114" s="1" t="n">
         <v>3360</v>
@@ -4771,13 +4755,13 @@
         <v>20</v>
       </c>
       <c r="I114" s="1" t="n">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="J114" s="1" t="n">
         <v>0.29</v>
       </c>
       <c r="K114" s="1" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="L114" s="1" t="n">
         <v>0.02</v>
@@ -4794,7 +4778,7 @@
         <v>48</v>
       </c>
       <c r="D115" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E115" s="1" t="n">
         <v>3360</v>
@@ -4812,7 +4796,7 @@
         <v>0.04</v>
       </c>
       <c r="K115" s="1" t="n">
-        <v>0.03</v>
+        <v>0.001</v>
       </c>
       <c r="L115" s="1" t="n">
         <v>0.002</v>
@@ -4829,10 +4813,10 @@
         <v>46</v>
       </c>
       <c r="D116" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E116" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G116" s="1" t="n">
         <v>30</v>
@@ -4841,13 +4825,13 @@
         <v>30</v>
       </c>
       <c r="I116" s="1" t="n">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="J116" s="1" t="n">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="K116" s="1" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L116" s="1" t="n">
         <v>0.01</v>
@@ -4864,10 +4848,10 @@
         <v>47</v>
       </c>
       <c r="D117" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E117" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G117" s="1" t="n">
         <v>20</v>
@@ -4876,16 +4860,16 @@
         <v>20</v>
       </c>
       <c r="I117" s="1" t="n">
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="J117" s="1" t="n">
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="K117" s="1" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="L117" s="1" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4899,10 +4883,10 @@
         <v>48</v>
       </c>
       <c r="D118" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E118" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G118" s="1" t="n">
         <v>50</v>
@@ -4911,13 +4895,13 @@
         <v>50</v>
       </c>
       <c r="I118" s="1" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="J118" s="1" t="n">
         <v>0.04</v>
       </c>
       <c r="K118" s="1" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="L118" s="1" t="n">
         <v>0.002</v>
@@ -4934,7 +4918,7 @@
         <v>46</v>
       </c>
       <c r="D119" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E119" s="1" t="n">
         <v>8760</v>
@@ -4946,7 +4930,7 @@
         <v>30</v>
       </c>
       <c r="I119" s="1" t="n">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="J119" s="1" t="n">
         <v>0.18</v>
@@ -4969,7 +4953,7 @@
         <v>47</v>
       </c>
       <c r="D120" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E120" s="1" t="n">
         <v>8760</v>
@@ -4981,13 +4965,13 @@
         <v>20</v>
       </c>
       <c r="I120" s="1" t="n">
-        <v>0.21</v>
+        <v>0.23</v>
       </c>
       <c r="J120" s="1" t="n">
         <v>0.26</v>
       </c>
       <c r="K120" s="1" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L120" s="1" t="n">
         <v>0.01</v>
@@ -5004,7 +4988,7 @@
         <v>48</v>
       </c>
       <c r="D121" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E121" s="1" t="n">
         <v>8760</v>
@@ -5039,10 +5023,10 @@
         <v>46</v>
       </c>
       <c r="D122" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E122" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G122" s="1" t="n">
         <v>30</v>
@@ -5051,16 +5035,16 @@
         <v>30</v>
       </c>
       <c r="I122" s="1" t="n">
-        <v>0.21</v>
+        <v>26.06</v>
       </c>
       <c r="J122" s="1" t="n">
-        <v>0.18</v>
+        <v>33.46</v>
       </c>
       <c r="K122" s="1" t="n">
-        <v>0.02</v>
+        <v>2.54</v>
       </c>
       <c r="L122" s="1" t="n">
-        <v>0.01</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5074,10 +5058,10 @@
         <v>47</v>
       </c>
       <c r="D123" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E123" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G123" s="1" t="n">
         <v>20</v>
@@ -5086,16 +5070,16 @@
         <v>20</v>
       </c>
       <c r="I123" s="1" t="n">
-        <v>0.23</v>
+        <v>22.76</v>
       </c>
       <c r="J123" s="1" t="n">
-        <v>0.26</v>
+        <v>24.19</v>
       </c>
       <c r="K123" s="1" t="n">
-        <v>0.02</v>
+        <v>2.22</v>
       </c>
       <c r="L123" s="1" t="n">
-        <v>0.01</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5109,10 +5093,10 @@
         <v>48</v>
       </c>
       <c r="D124" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E124" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G124" s="1" t="n">
         <v>50</v>
@@ -5121,16 +5105,16 @@
         <v>50</v>
       </c>
       <c r="I124" s="1" t="n">
-        <v>0.03</v>
+        <v>85.43</v>
       </c>
       <c r="J124" s="1" t="n">
-        <v>0.04</v>
+        <v>113.5</v>
       </c>
       <c r="K124" s="1" t="n">
-        <v>0.003</v>
+        <v>6.49</v>
       </c>
       <c r="L124" s="1" t="n">
-        <v>0.002</v>
+        <v>5.69</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5144,7 +5128,7 @@
         <v>46</v>
       </c>
       <c r="D125" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E125" s="1" t="n">
         <v>336</v>
@@ -5156,13 +5140,13 @@
         <v>30</v>
       </c>
       <c r="I125" s="1" t="n">
-        <v>26.06</v>
+        <v>26.35</v>
       </c>
       <c r="J125" s="1" t="n">
         <v>33.46</v>
       </c>
       <c r="K125" s="1" t="n">
-        <v>2.54</v>
+        <v>1.4</v>
       </c>
       <c r="L125" s="1" t="n">
         <v>1.3</v>
@@ -5179,7 +5163,7 @@
         <v>47</v>
       </c>
       <c r="D126" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E126" s="1" t="n">
         <v>336</v>
@@ -5191,13 +5175,13 @@
         <v>20</v>
       </c>
       <c r="I126" s="1" t="n">
-        <v>22.76</v>
+        <v>22.97</v>
       </c>
       <c r="J126" s="1" t="n">
         <v>24.19</v>
       </c>
       <c r="K126" s="1" t="n">
-        <v>2.22</v>
+        <v>1.33</v>
       </c>
       <c r="L126" s="1" t="n">
         <v>1.89</v>
@@ -5214,7 +5198,7 @@
         <v>48</v>
       </c>
       <c r="D127" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E127" s="1" t="n">
         <v>336</v>
@@ -5226,13 +5210,13 @@
         <v>50</v>
       </c>
       <c r="I127" s="1" t="n">
-        <v>85.43</v>
+        <v>119.62</v>
       </c>
       <c r="J127" s="1" t="n">
         <v>113.5</v>
       </c>
       <c r="K127" s="1" t="n">
-        <v>6.49</v>
+        <v>12.02</v>
       </c>
       <c r="L127" s="1" t="n">
         <v>5.69</v>
@@ -5249,10 +5233,10 @@
         <v>46</v>
       </c>
       <c r="D128" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E128" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G128" s="1" t="n">
         <v>30</v>
@@ -5261,16 +5245,16 @@
         <v>30</v>
       </c>
       <c r="I128" s="1" t="n">
-        <v>26.35</v>
+        <v>20.98</v>
       </c>
       <c r="J128" s="1" t="n">
-        <v>33.46</v>
+        <v>22.57</v>
       </c>
       <c r="K128" s="1" t="n">
-        <v>1.4</v>
+        <v>1.17</v>
       </c>
       <c r="L128" s="1" t="n">
-        <v>1.3</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5284,10 +5268,10 @@
         <v>47</v>
       </c>
       <c r="D129" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E129" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G129" s="1" t="n">
         <v>20</v>
@@ -5296,16 +5280,16 @@
         <v>20</v>
       </c>
       <c r="I129" s="1" t="n">
-        <v>22.97</v>
+        <v>38.23</v>
       </c>
       <c r="J129" s="1" t="n">
-        <v>24.19</v>
+        <v>39.59</v>
       </c>
       <c r="K129" s="1" t="n">
-        <v>1.33</v>
+        <v>3.72</v>
       </c>
       <c r="L129" s="1" t="n">
-        <v>1.89</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5319,10 +5303,10 @@
         <v>48</v>
       </c>
       <c r="D130" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E130" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G130" s="1" t="n">
         <v>50</v>
@@ -5331,16 +5315,16 @@
         <v>50</v>
       </c>
       <c r="I130" s="1" t="n">
-        <v>119.62</v>
+        <v>109.65</v>
       </c>
       <c r="J130" s="1" t="n">
-        <v>113.5</v>
+        <v>122.68</v>
       </c>
       <c r="K130" s="1" t="n">
-        <v>12.02</v>
+        <v>3.67</v>
       </c>
       <c r="L130" s="1" t="n">
-        <v>5.69</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5354,7 +5338,7 @@
         <v>46</v>
       </c>
       <c r="D131" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E131" s="1" t="n">
         <v>3360</v>
@@ -5366,13 +5350,13 @@
         <v>30</v>
       </c>
       <c r="I131" s="1" t="n">
-        <v>20.98</v>
+        <v>36.1</v>
       </c>
       <c r="J131" s="1" t="n">
         <v>22.57</v>
       </c>
       <c r="K131" s="1" t="n">
-        <v>1.17</v>
+        <v>3.78</v>
       </c>
       <c r="L131" s="1" t="n">
         <v>2.63</v>
@@ -5389,7 +5373,7 @@
         <v>47</v>
       </c>
       <c r="D132" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E132" s="1" t="n">
         <v>3360</v>
@@ -5401,13 +5385,13 @@
         <v>20</v>
       </c>
       <c r="I132" s="1" t="n">
-        <v>38.23</v>
+        <v>28.22</v>
       </c>
       <c r="J132" s="1" t="n">
         <v>39.59</v>
       </c>
       <c r="K132" s="1" t="n">
-        <v>3.72</v>
+        <v>3.09</v>
       </c>
       <c r="L132" s="1" t="n">
         <v>4.1</v>
@@ -5424,7 +5408,7 @@
         <v>48</v>
       </c>
       <c r="D133" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E133" s="1" t="n">
         <v>3360</v>
@@ -5436,13 +5420,13 @@
         <v>50</v>
       </c>
       <c r="I133" s="1" t="n">
-        <v>109.65</v>
+        <v>89.83</v>
       </c>
       <c r="J133" s="1" t="n">
         <v>122.68</v>
       </c>
       <c r="K133" s="1" t="n">
-        <v>3.67</v>
+        <v>6.29</v>
       </c>
       <c r="L133" s="1" t="n">
         <v>4.7</v>
@@ -5459,10 +5443,10 @@
         <v>46</v>
       </c>
       <c r="D134" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E134" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G134" s="1" t="n">
         <v>30</v>
@@ -5471,16 +5455,16 @@
         <v>30</v>
       </c>
       <c r="I134" s="1" t="n">
-        <v>36.1</v>
+        <v>24.18</v>
       </c>
       <c r="J134" s="1" t="n">
-        <v>22.57</v>
+        <v>36.07</v>
       </c>
       <c r="K134" s="1" t="n">
-        <v>3.78</v>
+        <v>1.63</v>
       </c>
       <c r="L134" s="1" t="n">
-        <v>2.63</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5494,10 +5478,10 @@
         <v>47</v>
       </c>
       <c r="D135" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E135" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G135" s="1" t="n">
         <v>20</v>
@@ -5506,16 +5490,16 @@
         <v>20</v>
       </c>
       <c r="I135" s="1" t="n">
-        <v>28.22</v>
+        <v>24.26</v>
       </c>
       <c r="J135" s="1" t="n">
-        <v>39.59</v>
+        <v>28.52</v>
       </c>
       <c r="K135" s="1" t="n">
-        <v>3.09</v>
+        <v>1.53</v>
       </c>
       <c r="L135" s="1" t="n">
-        <v>4.1</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5529,10 +5513,10 @@
         <v>48</v>
       </c>
       <c r="D136" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E136" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G136" s="1" t="n">
         <v>50</v>
@@ -5541,16 +5525,16 @@
         <v>50</v>
       </c>
       <c r="I136" s="1" t="n">
-        <v>89.83</v>
+        <v>90.54</v>
       </c>
       <c r="J136" s="1" t="n">
-        <v>122.68</v>
+        <v>101.39</v>
       </c>
       <c r="K136" s="1" t="n">
-        <v>6.29</v>
+        <v>2</v>
       </c>
       <c r="L136" s="1" t="n">
-        <v>4.7</v>
+        <v>5.09</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5564,7 +5548,7 @@
         <v>46</v>
       </c>
       <c r="D137" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E137" s="1" t="n">
         <v>8760</v>
@@ -5576,13 +5560,13 @@
         <v>30</v>
       </c>
       <c r="I137" s="1" t="n">
-        <v>24.18</v>
+        <v>34.16</v>
       </c>
       <c r="J137" s="1" t="n">
         <v>36.07</v>
       </c>
       <c r="K137" s="1" t="n">
-        <v>1.63</v>
+        <v>3.39</v>
       </c>
       <c r="L137" s="1" t="n">
         <v>3.17</v>
@@ -5599,7 +5583,7 @@
         <v>47</v>
       </c>
       <c r="D138" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E138" s="1" t="n">
         <v>8760</v>
@@ -5611,13 +5595,13 @@
         <v>20</v>
       </c>
       <c r="I138" s="1" t="n">
-        <v>24.26</v>
+        <v>24.13</v>
       </c>
       <c r="J138" s="1" t="n">
         <v>28.52</v>
       </c>
       <c r="K138" s="1" t="n">
-        <v>1.53</v>
+        <v>0.82</v>
       </c>
       <c r="L138" s="1" t="n">
         <v>1.29</v>
@@ -5634,7 +5618,7 @@
         <v>48</v>
       </c>
       <c r="D139" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E139" s="1" t="n">
         <v>8760</v>
@@ -5646,13 +5630,13 @@
         <v>50</v>
       </c>
       <c r="I139" s="1" t="n">
-        <v>90.54</v>
+        <v>130.87</v>
       </c>
       <c r="J139" s="1" t="n">
         <v>101.39</v>
       </c>
       <c r="K139" s="1" t="n">
-        <v>2</v>
+        <v>10.18</v>
       </c>
       <c r="L139" s="1" t="n">
         <v>5.09</v>
@@ -5669,10 +5653,10 @@
         <v>46</v>
       </c>
       <c r="D140" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E140" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G140" s="1" t="n">
         <v>30</v>
@@ -5681,16 +5665,16 @@
         <v>30</v>
       </c>
       <c r="I140" s="1" t="n">
-        <v>34.16</v>
+        <v>3.97</v>
       </c>
       <c r="J140" s="1" t="n">
-        <v>36.07</v>
+        <v>4.45</v>
       </c>
       <c r="K140" s="1" t="n">
-        <v>3.39</v>
+        <v>0.51</v>
       </c>
       <c r="L140" s="1" t="n">
-        <v>3.17</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5704,10 +5688,10 @@
         <v>47</v>
       </c>
       <c r="D141" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E141" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G141" s="1" t="n">
         <v>20</v>
@@ -5716,16 +5700,16 @@
         <v>20</v>
       </c>
       <c r="I141" s="1" t="n">
-        <v>24.13</v>
+        <v>3.7</v>
       </c>
       <c r="J141" s="1" t="n">
-        <v>28.52</v>
+        <v>5.87</v>
       </c>
       <c r="K141" s="1" t="n">
-        <v>0.82</v>
+        <v>0.63</v>
       </c>
       <c r="L141" s="1" t="n">
-        <v>1.29</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5739,10 +5723,10 @@
         <v>48</v>
       </c>
       <c r="D142" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E142" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G142" s="1" t="n">
         <v>50</v>
@@ -5751,16 +5735,16 @@
         <v>50</v>
       </c>
       <c r="I142" s="1" t="n">
-        <v>130.87</v>
+        <v>3.07</v>
       </c>
       <c r="J142" s="1" t="n">
-        <v>101.39</v>
+        <v>4.13</v>
       </c>
       <c r="K142" s="1" t="n">
-        <v>10.18</v>
+        <v>0.3</v>
       </c>
       <c r="L142" s="1" t="n">
-        <v>5.09</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5774,7 +5758,7 @@
         <v>46</v>
       </c>
       <c r="D143" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E143" s="1" t="n">
         <v>336</v>
@@ -5786,13 +5770,13 @@
         <v>30</v>
       </c>
       <c r="I143" s="1" t="n">
-        <v>3.97</v>
+        <v>5.29</v>
       </c>
       <c r="J143" s="1" t="n">
         <v>4.45</v>
       </c>
       <c r="K143" s="1" t="n">
-        <v>0.51</v>
+        <v>0.32</v>
       </c>
       <c r="L143" s="1" t="n">
         <v>0.49</v>
@@ -5809,7 +5793,7 @@
         <v>47</v>
       </c>
       <c r="D144" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E144" s="1" t="n">
         <v>336</v>
@@ -5821,13 +5805,13 @@
         <v>20</v>
       </c>
       <c r="I144" s="1" t="n">
-        <v>3.7</v>
+        <v>4.99</v>
       </c>
       <c r="J144" s="1" t="n">
         <v>5.87</v>
       </c>
       <c r="K144" s="1" t="n">
-        <v>0.63</v>
+        <v>1.03</v>
       </c>
       <c r="L144" s="1" t="n">
         <v>1.23</v>
@@ -5844,7 +5828,7 @@
         <v>48</v>
       </c>
       <c r="D145" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E145" s="1" t="n">
         <v>336</v>
@@ -5856,13 +5840,13 @@
         <v>50</v>
       </c>
       <c r="I145" s="1" t="n">
-        <v>3.07</v>
+        <v>3.63</v>
       </c>
       <c r="J145" s="1" t="n">
         <v>4.13</v>
       </c>
       <c r="K145" s="1" t="n">
-        <v>0.3</v>
+        <v>0.38</v>
       </c>
       <c r="L145" s="1" t="n">
         <v>0.5</v>
@@ -5879,10 +5863,10 @@
         <v>46</v>
       </c>
       <c r="D146" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E146" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G146" s="1" t="n">
         <v>30</v>
@@ -5891,16 +5875,16 @@
         <v>30</v>
       </c>
       <c r="I146" s="1" t="n">
-        <v>5.29</v>
+        <v>3.61</v>
       </c>
       <c r="J146" s="1" t="n">
-        <v>4.45</v>
+        <v>5.46</v>
       </c>
       <c r="K146" s="1" t="n">
-        <v>0.32</v>
+        <v>0.58</v>
       </c>
       <c r="L146" s="1" t="n">
-        <v>0.49</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5914,10 +5898,10 @@
         <v>47</v>
       </c>
       <c r="D147" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E147" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G147" s="1" t="n">
         <v>20</v>
@@ -5926,16 +5910,16 @@
         <v>20</v>
       </c>
       <c r="I147" s="1" t="n">
-        <v>4.99</v>
+        <v>2.73</v>
       </c>
       <c r="J147" s="1" t="n">
-        <v>5.87</v>
+        <v>2.11</v>
       </c>
       <c r="K147" s="1" t="n">
-        <v>1.03</v>
+        <v>0.63</v>
       </c>
       <c r="L147" s="1" t="n">
-        <v>1.23</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5949,10 +5933,10 @@
         <v>48</v>
       </c>
       <c r="D148" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E148" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G148" s="1" t="n">
         <v>50</v>
@@ -5961,16 +5945,16 @@
         <v>50</v>
       </c>
       <c r="I148" s="1" t="n">
-        <v>3.63</v>
+        <v>4.69</v>
       </c>
       <c r="J148" s="1" t="n">
-        <v>4.13</v>
+        <v>3.71</v>
       </c>
       <c r="K148" s="1" t="n">
-        <v>0.38</v>
+        <v>0.5</v>
       </c>
       <c r="L148" s="1" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5984,7 +5968,7 @@
         <v>46</v>
       </c>
       <c r="D149" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E149" s="1" t="n">
         <v>3360</v>
@@ -5996,13 +5980,13 @@
         <v>30</v>
       </c>
       <c r="I149" s="1" t="n">
-        <v>3.61</v>
+        <v>4.64</v>
       </c>
       <c r="J149" s="1" t="n">
         <v>5.46</v>
       </c>
       <c r="K149" s="1" t="n">
-        <v>0.58</v>
+        <v>0.31</v>
       </c>
       <c r="L149" s="1" t="n">
         <v>0.37</v>
@@ -6019,7 +6003,7 @@
         <v>47</v>
       </c>
       <c r="D150" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E150" s="1" t="n">
         <v>3360</v>
@@ -6031,13 +6015,13 @@
         <v>20</v>
       </c>
       <c r="I150" s="1" t="n">
-        <v>2.73</v>
+        <v>3.38</v>
       </c>
       <c r="J150" s="1" t="n">
         <v>2.11</v>
       </c>
       <c r="K150" s="1" t="n">
-        <v>0.63</v>
+        <v>0.5</v>
       </c>
       <c r="L150" s="1" t="n">
         <v>0.25</v>
@@ -6054,7 +6038,7 @@
         <v>48</v>
       </c>
       <c r="D151" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E151" s="1" t="n">
         <v>3360</v>
@@ -6066,13 +6050,13 @@
         <v>50</v>
       </c>
       <c r="I151" s="1" t="n">
-        <v>4.69</v>
+        <v>6.52</v>
       </c>
       <c r="J151" s="1" t="n">
         <v>3.71</v>
       </c>
       <c r="K151" s="1" t="n">
-        <v>0.5</v>
+        <v>0.58</v>
       </c>
       <c r="L151" s="1" t="n">
         <v>0.3</v>
@@ -6089,10 +6073,10 @@
         <v>46</v>
       </c>
       <c r="D152" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E152" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G152" s="1" t="n">
         <v>30</v>
@@ -6101,16 +6085,16 @@
         <v>30</v>
       </c>
       <c r="I152" s="1" t="n">
-        <v>4.64</v>
+        <v>4.14</v>
       </c>
       <c r="J152" s="1" t="n">
-        <v>5.46</v>
+        <v>5.41</v>
       </c>
       <c r="K152" s="1" t="n">
-        <v>0.31</v>
+        <v>0.41</v>
       </c>
       <c r="L152" s="1" t="n">
-        <v>0.37</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6124,10 +6108,10 @@
         <v>47</v>
       </c>
       <c r="D153" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E153" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G153" s="1" t="n">
         <v>20</v>
@@ -6136,16 +6120,16 @@
         <v>20</v>
       </c>
       <c r="I153" s="1" t="n">
-        <v>3.38</v>
+        <v>4.85</v>
       </c>
       <c r="J153" s="1" t="n">
-        <v>2.11</v>
+        <v>4.13</v>
       </c>
       <c r="K153" s="1" t="n">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="L153" s="1" t="n">
-        <v>0.25</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6159,10 +6143,10 @@
         <v>48</v>
       </c>
       <c r="D154" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E154" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G154" s="1" t="n">
         <v>50</v>
@@ -6171,16 +6155,16 @@
         <v>50</v>
       </c>
       <c r="I154" s="1" t="n">
-        <v>6.52</v>
+        <v>2.56</v>
       </c>
       <c r="J154" s="1" t="n">
-        <v>3.71</v>
+        <v>6.08</v>
       </c>
       <c r="K154" s="1" t="n">
-        <v>0.58</v>
+        <v>0.25</v>
       </c>
       <c r="L154" s="1" t="n">
-        <v>0.3</v>
+        <v>1.63</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6194,7 +6178,7 @@
         <v>46</v>
       </c>
       <c r="D155" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E155" s="1" t="n">
         <v>8760</v>
@@ -6206,13 +6190,13 @@
         <v>30</v>
       </c>
       <c r="I155" s="1" t="n">
-        <v>4.14</v>
+        <v>3.75</v>
       </c>
       <c r="J155" s="1" t="n">
         <v>5.41</v>
       </c>
       <c r="K155" s="1" t="n">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="L155" s="1" t="n">
         <v>0.58</v>
@@ -6229,7 +6213,7 @@
         <v>47</v>
       </c>
       <c r="D156" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E156" s="1" t="n">
         <v>8760</v>
@@ -6241,13 +6225,13 @@
         <v>20</v>
       </c>
       <c r="I156" s="1" t="n">
-        <v>4.85</v>
+        <v>7.54</v>
       </c>
       <c r="J156" s="1" t="n">
         <v>4.13</v>
       </c>
       <c r="K156" s="1" t="n">
-        <v>0.77</v>
+        <v>1.75</v>
       </c>
       <c r="L156" s="1" t="n">
         <v>0.66</v>
@@ -6264,7 +6248,7 @@
         <v>48</v>
       </c>
       <c r="D157" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E157" s="1" t="n">
         <v>8760</v>
@@ -6276,13 +6260,13 @@
         <v>50</v>
       </c>
       <c r="I157" s="1" t="n">
-        <v>2.56</v>
+        <v>9.34</v>
       </c>
       <c r="J157" s="1" t="n">
         <v>6.08</v>
       </c>
       <c r="K157" s="1" t="n">
-        <v>0.25</v>
+        <v>1.31</v>
       </c>
       <c r="L157" s="1" t="n">
         <v>1.63</v>
@@ -6299,10 +6283,10 @@
         <v>46</v>
       </c>
       <c r="D158" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E158" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G158" s="1" t="n">
         <v>30</v>
@@ -6311,16 +6295,16 @@
         <v>30</v>
       </c>
       <c r="I158" s="1" t="n">
-        <v>3.75</v>
+        <v>0.41</v>
       </c>
       <c r="J158" s="1" t="n">
-        <v>5.41</v>
+        <v>0.4</v>
       </c>
       <c r="K158" s="1" t="n">
-        <v>0.39</v>
+        <v>0.07</v>
       </c>
       <c r="L158" s="1" t="n">
-        <v>0.58</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6334,10 +6318,10 @@
         <v>47</v>
       </c>
       <c r="D159" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E159" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G159" s="1" t="n">
         <v>20</v>
@@ -6346,16 +6330,16 @@
         <v>20</v>
       </c>
       <c r="I159" s="1" t="n">
-        <v>7.54</v>
+        <v>0.28</v>
       </c>
       <c r="J159" s="1" t="n">
-        <v>4.13</v>
+        <v>0.27</v>
       </c>
       <c r="K159" s="1" t="n">
-        <v>1.75</v>
+        <v>0.02</v>
       </c>
       <c r="L159" s="1" t="n">
-        <v>0.66</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6369,10 +6353,10 @@
         <v>48</v>
       </c>
       <c r="D160" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E160" s="1" t="n">
-        <v>8760</v>
+        <v>336</v>
       </c>
       <c r="G160" s="1" t="n">
         <v>50</v>
@@ -6381,16 +6365,16 @@
         <v>50</v>
       </c>
       <c r="I160" s="1" t="n">
-        <v>9.34</v>
+        <v>1.78</v>
       </c>
       <c r="J160" s="1" t="n">
-        <v>6.08</v>
+        <v>2.28</v>
       </c>
       <c r="K160" s="1" t="n">
-        <v>1.31</v>
+        <v>0.16</v>
       </c>
       <c r="L160" s="1" t="n">
-        <v>1.63</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,7 +6388,7 @@
         <v>46</v>
       </c>
       <c r="D161" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E161" s="1" t="n">
         <v>336</v>
@@ -6416,13 +6400,13 @@
         <v>30</v>
       </c>
       <c r="I161" s="1" t="n">
-        <v>0.41</v>
+        <v>0.72</v>
       </c>
       <c r="J161" s="1" t="n">
         <v>0.4</v>
       </c>
       <c r="K161" s="1" t="n">
-        <v>0.07</v>
+        <v>0.16</v>
       </c>
       <c r="L161" s="1" t="n">
         <v>0.07</v>
@@ -6439,7 +6423,7 @@
         <v>47</v>
       </c>
       <c r="D162" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E162" s="1" t="n">
         <v>336</v>
@@ -6451,13 +6435,13 @@
         <v>20</v>
       </c>
       <c r="I162" s="1" t="n">
-        <v>0.28</v>
+        <v>0.18</v>
       </c>
       <c r="J162" s="1" t="n">
         <v>0.27</v>
       </c>
       <c r="K162" s="1" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="L162" s="1" t="n">
         <v>0.02</v>
@@ -6474,7 +6458,7 @@
         <v>48</v>
       </c>
       <c r="D163" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E163" s="1" t="n">
         <v>336</v>
@@ -6486,13 +6470,13 @@
         <v>50</v>
       </c>
       <c r="I163" s="1" t="n">
-        <v>1.78</v>
+        <v>3.15</v>
       </c>
       <c r="J163" s="1" t="n">
         <v>2.28</v>
       </c>
       <c r="K163" s="1" t="n">
-        <v>0.16</v>
+        <v>0.4</v>
       </c>
       <c r="L163" s="1" t="n">
         <v>0.1</v>
@@ -6509,10 +6493,10 @@
         <v>46</v>
       </c>
       <c r="D164" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E164" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G164" s="1" t="n">
         <v>30</v>
@@ -6521,16 +6505,16 @@
         <v>30</v>
       </c>
       <c r="I164" s="1" t="n">
-        <v>0.72</v>
+        <v>0.69</v>
       </c>
       <c r="J164" s="1" t="n">
-        <v>0.4</v>
+        <v>0.88</v>
       </c>
       <c r="K164" s="1" t="n">
-        <v>0.16</v>
+        <v>0.11</v>
       </c>
       <c r="L164" s="1" t="n">
-        <v>0.07</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6544,10 +6528,10 @@
         <v>47</v>
       </c>
       <c r="D165" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E165" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G165" s="1" t="n">
         <v>20</v>
@@ -6556,16 +6540,16 @@
         <v>20</v>
       </c>
       <c r="I165" s="1" t="n">
-        <v>0.18</v>
+        <v>0.29</v>
       </c>
       <c r="J165" s="1" t="n">
-        <v>0.27</v>
+        <v>0.22</v>
       </c>
       <c r="K165" s="1" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="L165" s="1" t="n">
-        <v>0.02</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6579,10 +6563,10 @@
         <v>48</v>
       </c>
       <c r="D166" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E166" s="1" t="n">
-        <v>336</v>
+        <v>3360</v>
       </c>
       <c r="G166" s="1" t="n">
         <v>50</v>
@@ -6591,16 +6575,16 @@
         <v>50</v>
       </c>
       <c r="I166" s="1" t="n">
-        <v>3.15</v>
+        <v>1.7</v>
       </c>
       <c r="J166" s="1" t="n">
-        <v>2.28</v>
+        <v>1.72</v>
       </c>
       <c r="K166" s="1" t="n">
-        <v>0.4</v>
+        <v>0.16</v>
       </c>
       <c r="L166" s="1" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6614,7 +6598,7 @@
         <v>46</v>
       </c>
       <c r="D167" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E167" s="1" t="n">
         <v>3360</v>
@@ -6626,13 +6610,13 @@
         <v>30</v>
       </c>
       <c r="I167" s="1" t="n">
-        <v>0.69</v>
+        <v>1.02</v>
       </c>
       <c r="J167" s="1" t="n">
         <v>0.88</v>
       </c>
       <c r="K167" s="1" t="n">
-        <v>0.11</v>
+        <v>0.15</v>
       </c>
       <c r="L167" s="1" t="n">
         <v>0.14</v>
@@ -6649,7 +6633,7 @@
         <v>47</v>
       </c>
       <c r="D168" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E168" s="1" t="n">
         <v>3360</v>
@@ -6661,13 +6645,13 @@
         <v>20</v>
       </c>
       <c r="I168" s="1" t="n">
-        <v>0.29</v>
+        <v>0.19</v>
       </c>
       <c r="J168" s="1" t="n">
         <v>0.22</v>
       </c>
       <c r="K168" s="1" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="L168" s="1" t="n">
         <v>0.07</v>
@@ -6684,7 +6668,7 @@
         <v>48</v>
       </c>
       <c r="D169" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E169" s="1" t="n">
         <v>3360</v>
@@ -6696,13 +6680,13 @@
         <v>50</v>
       </c>
       <c r="I169" s="1" t="n">
-        <v>1.7</v>
+        <v>2.44</v>
       </c>
       <c r="J169" s="1" t="n">
         <v>1.72</v>
       </c>
       <c r="K169" s="1" t="n">
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="L169" s="1" t="n">
         <v>0.15</v>
@@ -6719,10 +6703,10 @@
         <v>46</v>
       </c>
       <c r="D170" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E170" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G170" s="1" t="n">
         <v>30</v>
@@ -6731,16 +6715,16 @@
         <v>30</v>
       </c>
       <c r="I170" s="1" t="n">
-        <v>1.02</v>
+        <v>0.47</v>
       </c>
       <c r="J170" s="1" t="n">
-        <v>0.88</v>
+        <v>1.09</v>
       </c>
       <c r="K170" s="1" t="n">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="L170" s="1" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6754,10 +6738,10 @@
         <v>47</v>
       </c>
       <c r="D171" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E171" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G171" s="1" t="n">
         <v>20</v>
@@ -6766,16 +6750,16 @@
         <v>20</v>
       </c>
       <c r="I171" s="1" t="n">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="J171" s="1" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="K171" s="1" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="L171" s="1" t="n">
-        <v>0.07</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6789,10 +6773,10 @@
         <v>48</v>
       </c>
       <c r="D172" s="1" t="n">
-        <v>1</v>
+        <v>0.07</v>
       </c>
       <c r="E172" s="1" t="n">
-        <v>3360</v>
+        <v>8760</v>
       </c>
       <c r="G172" s="1" t="n">
         <v>50</v>
@@ -6801,16 +6785,16 @@
         <v>50</v>
       </c>
       <c r="I172" s="1" t="n">
-        <v>2.44</v>
+        <v>2.5</v>
       </c>
       <c r="J172" s="1" t="n">
-        <v>1.72</v>
+        <v>2.63</v>
       </c>
       <c r="K172" s="1" t="n">
-        <v>0.24</v>
+        <v>0.3</v>
       </c>
       <c r="L172" s="1" t="n">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6824,7 +6808,7 @@
         <v>46</v>
       </c>
       <c r="D173" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E173" s="1" t="n">
         <v>8760</v>
@@ -6836,13 +6820,13 @@
         <v>30</v>
       </c>
       <c r="I173" s="1" t="n">
-        <v>0.47</v>
+        <v>1.26</v>
       </c>
       <c r="J173" s="1" t="n">
         <v>1.09</v>
       </c>
       <c r="K173" s="1" t="n">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="L173" s="1" t="n">
         <v>0.16</v>
@@ -6859,7 +6843,7 @@
         <v>47</v>
       </c>
       <c r="D174" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E174" s="1" t="n">
         <v>8760</v>
@@ -6871,13 +6855,13 @@
         <v>20</v>
       </c>
       <c r="I174" s="1" t="n">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="J174" s="1" t="n">
         <v>0.21</v>
       </c>
       <c r="K174" s="1" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="L174" s="1" t="n">
         <v>0.05</v>
@@ -6894,7 +6878,7 @@
         <v>48</v>
       </c>
       <c r="D175" s="1" t="n">
-        <v>0.07</v>
+        <v>1</v>
       </c>
       <c r="E175" s="1" t="n">
         <v>8760</v>
@@ -6906,13 +6890,13 @@
         <v>50</v>
       </c>
       <c r="I175" s="1" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J175" s="1" t="n">
         <v>2.63</v>
       </c>
       <c r="K175" s="1" t="n">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="L175" s="1" t="n">
         <v>0.08</v>
@@ -6920,189 +6904,70 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D176" s="1" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E176" s="1" t="n">
-        <v>8760</v>
+        <v>0.6666</v>
       </c>
       <c r="G176" s="1" t="n">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="H176" s="1" t="n">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="I176" s="1" t="n">
-        <v>1.26</v>
+        <v>90</v>
       </c>
       <c r="J176" s="1" t="n">
-        <v>1.09</v>
+        <v>86.6</v>
       </c>
       <c r="K176" s="1" t="n">
-        <v>0.12</v>
+        <v>10</v>
       </c>
       <c r="L176" s="1" t="n">
-        <v>0.16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D177" s="1" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E177" s="1" t="n">
-        <v>8760</v>
+        <v>1176</v>
       </c>
       <c r="G177" s="1" t="n">
-        <v>20</v>
+        <v>81</v>
       </c>
       <c r="H177" s="1" t="n">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="I177" s="1" t="n">
-        <v>0.15</v>
+        <v>78.6</v>
       </c>
       <c r="J177" s="1" t="n">
-        <v>0.21</v>
+        <v>95.2</v>
       </c>
       <c r="K177" s="1" t="n">
-        <v>0.02</v>
+        <v>22.5</v>
       </c>
       <c r="L177" s="1" t="n">
-        <v>0.05</v>
+        <v>19</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D178" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E178" s="1" t="n">
-        <v>8760</v>
-      </c>
-      <c r="G178" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="H178" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="I178" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J178" s="1" t="n">
-        <v>2.63</v>
-      </c>
-      <c r="K178" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="L178" s="1" t="n">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E179" s="1" t="n">
-        <v>0.6666</v>
-      </c>
-      <c r="G179" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="H179" s="1" t="n">
-        <v>99</v>
-      </c>
-      <c r="I179" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="J179" s="1" t="n">
-        <v>86.6</v>
-      </c>
-      <c r="K179" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="L179" s="1" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C180" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E180" s="1" t="n">
-        <v>1176</v>
-      </c>
-      <c r="G180" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="H180" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="I180" s="1" t="n">
-        <v>78.6</v>
-      </c>
-      <c r="J180" s="1" t="n">
-        <v>95.2</v>
-      </c>
-      <c r="K180" s="1" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="L180" s="1" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D181" s="1" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="E181" s="1" t="n">
-        <v>200</v>
-      </c>
+      <c r="E178" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>